<commit_message>
l. Plotted rought plots
</commit_message>
<xml_diff>
--- a/Notebooks/data/base_function.xlsx
+++ b/Notebooks/data/base_function.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosreyes/Desktop/Academics/postdoc/confirm/python/optosurf/Notebooks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EC4AD0-0942-C541-8DF1-BA7BAFF49D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F7A91E-2705-DB4F-8A81-C2EA7BDEC8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39180" yWindow="260" windowWidth="27640" windowHeight="16940" xr2:uid="{6589966E-8578-6742-BE7F-85CD1E238E1B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20020" activeTab="1" xr2:uid="{6589966E-8578-6742-BE7F-85CD1E238E1B}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="1" r:id="rId1"/>
@@ -393,7 +393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D7E307-E92B-544A-A3D9-86E545925D7E}">
   <dimension ref="A1:W33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+    <sheetView zoomScale="85" workbookViewId="0">
       <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
@@ -2751,7 +2751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D419D00-A5DE-0340-B4D7-3252F843C6CB}">
   <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>